<commit_message>
pokemon data loader added
</commit_message>
<xml_diff>
--- a/resources/testdata/pokemon-test-data.xlsx
+++ b/resources/testdata/pokemon-test-data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://monnetpe-my.sharepoint.com/personal/bruno_barros_monnetpayments_com/Documents/Documentos/Cosas QA/Entrevista/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silsop\Desktop\Monnet Payments\challenge\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D49B7E23-8659-401E-A2A4-FE54DD71A3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="7956" yWindow="1044" windowWidth="11316" windowHeight="11316" xr2:uid="{84F1231F-6146-4E51-AA5A-5DDC7EDEF056}"/>
+    <workbookView xWindow="7950" yWindow="1050" windowWidth="11310" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="GET pokemon" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -433,16 +432,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4282182B-0C5A-4F61-AEAA-4FEDC72228A7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>